<commit_message>
initialization of bet.hu download started
</commit_message>
<xml_diff>
--- a/Instruments/tickers.xlsx
+++ b/Instruments/tickers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="121">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">First trading</t>
   </si>
   <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
     <t xml:space="preserve">4iG Nyrt.</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">HUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bet.hu/oldalak/adatletoltes</t>
   </si>
   <si>
     <t xml:space="preserve">Otp Bank Nyrt.</t>
@@ -452,9 +458,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -474,10 +484,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -487,7 +497,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.38"/>
@@ -516,579 +526,700 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>280000010</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>819424824</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1042742543</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>186374860</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>701646050</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>21054655</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>13473446</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>66000010</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>17693734</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>2000000</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>6074441</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>3050421</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>7500000</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>101815648</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>100000000</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>60713000</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>29815766</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>35852000</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>49483025</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>19386274</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>89</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>14794650</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>93</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>47371419</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>270261400</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>287024440</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>3438787</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>10631674</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>113</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>14601279</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>94428260</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G4" r:id="rId3" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G5" r:id="rId4" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G6" r:id="rId5" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G7" r:id="rId6" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G8" r:id="rId7" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G9" r:id="rId8" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G10" r:id="rId9" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G11" r:id="rId10" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G12" r:id="rId11" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G13" r:id="rId12" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G14" r:id="rId13" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G15" r:id="rId14" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G16" r:id="rId15" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G17" r:id="rId16" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G18" r:id="rId17" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G19" r:id="rId18" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G20" r:id="rId19" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G21" r:id="rId20" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G22" r:id="rId21" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G23" r:id="rId22" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G24" r:id="rId23" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G25" r:id="rId24" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G26" r:id="rId25" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G27" r:id="rId26" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G28" r:id="rId27" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G29" r:id="rId28" display="https://bet.hu/oldalak/adatletoltes"/>
+    <hyperlink ref="G30" r:id="rId29" display="https://bet.hu/oldalak/adatletoltes"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
cannot figure out the instrument select part
</commit_message>
<xml_diff>
--- a/Instruments/tickers.xlsx
+++ b/Instruments/tickers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="126">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">URL</t>
   </si>
   <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
     <t xml:space="preserve">4iG Nyrt.</t>
   </si>
   <si>
@@ -52,9 +55,18 @@
     <t xml:space="preserve">HUF</t>
   </si>
   <si>
+    <t xml:space="preserve">HU0000167788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004.09.22.</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://bet.hu/oldalak/adatletoltes</t>
   </si>
   <si>
+    <t xml:space="preserve">W_RESZVENYA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Otp Bank Nyrt.</t>
   </si>
   <si>
@@ -185,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">1998.12.15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W_RESZVENYB</t>
   </si>
   <si>
     <t xml:space="preserve">Észak-magyarországi Áramszolgáltató</t>
@@ -484,10 +499,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -529,663 +544,762 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>94000000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>280000010</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>819424824</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1042742543</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>186374860</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>701646050</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>21054655</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>13473446</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>66000010</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>17693734</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>2000000</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>6074441</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>3050421</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>7500000</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>101815648</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>100000000</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>60713000</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>29815766</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>35852000</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>49483025</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>19386274</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>14794650</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>47371419</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>270261400</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>287024440</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>3438787</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>10631674</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>14601279</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>94428260</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
request version of data download close to work
</commit_message>
<xml_diff>
--- a/Instruments/tickers.xlsx
+++ b/Instruments/tickers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="128">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Category</t>
   </si>
   <si>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
     <t xml:space="preserve">4iG Nyrt.</t>
   </si>
   <si>
@@ -329,6 +332,9 @@
   </si>
   <si>
     <t xml:space="preserve">2010.07.02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">AutoWallis</t>
@@ -499,10 +505,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -547,759 +553,852 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>94000000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>3564</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>280000010</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>528</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>819424824</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>518</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1042742543</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>511</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>186374860</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>608</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>701646050</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>540</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>21054655</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>546</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>13473446</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>604</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>66000010</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>3263</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>17693734</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>11141</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>2000000</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>639</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>6074441</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>703</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>3050421</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>702</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>7500000</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>4664</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>101815648</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>748</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>100000000</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>12625</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>60713000</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>6005</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>29815766</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>477</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>35852000</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>6461</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>49483025</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>6907</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>19386274</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>6494</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>14794650</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>4042</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>47371419</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>6329</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>270261400</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>8208</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>287024440</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>3438787</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>9864</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>10631674</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>4338</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>14601279</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>7217</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>94428260</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>6515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>